<commit_message>
updates for Rev1B boards, pinout changes on J5 and J8
</commit_message>
<xml_diff>
--- a/echopilot_carrier_r1_bom.xlsx
+++ b/echopilot_carrier_r1_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\horizon31\boards\EchoPilot AI Carrier Board - Public\gerbers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BradStinson\Documents\EchoMAV\Boards\EchoPilot AI Carrier Board - Public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913DC9A-D779-4E55-BC3F-E9D84161A872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D2AE54-FF86-43D2-BA42-DF751E40A42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="4365" windowWidth="38895" windowHeight="19635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="34500" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pixc4-jetson-universal-carrier" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="368">
   <si>
     <t>Item</t>
   </si>
@@ -1121,6 +1121,9 @@
   </si>
   <si>
     <t>Keystone 5015 Test Point</t>
+  </si>
+  <si>
+    <t>Possible Sub: SRP1038A-8R2M</t>
   </si>
 </sst>
 </file>
@@ -1981,31 +1984,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.26953125" customWidth="1"/>
     <col min="4" max="4" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2100,7 +2103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2123,7 +2126,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2146,7 +2149,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>13</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2376,7 +2379,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2491,7 +2494,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2606,7 +2609,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2629,7 +2632,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2652,7 +2655,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2675,7 +2678,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>29</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>30</v>
       </c>
@@ -2721,7 +2724,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>31</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>32</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>33</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>34</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>35</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>36</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>37</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>38</v>
       </c>
@@ -2905,7 +2908,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>39</v>
       </c>
@@ -2928,7 +2931,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>40</v>
       </c>
@@ -2951,7 +2954,7 @@
         <v>532617010</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>41</v>
       </c>
@@ -2974,7 +2977,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>42</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>43</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>44</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>45</v>
       </c>
@@ -3066,7 +3069,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>46</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>47</v>
       </c>
@@ -3112,7 +3115,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>48</v>
       </c>
@@ -3135,7 +3138,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>49</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>50</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>51</v>
       </c>
@@ -3204,7 +3207,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>52</v>
       </c>
@@ -3226,8 +3229,11 @@
       <c r="G56" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>53</v>
       </c>
@@ -3250,7 +3256,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>54</v>
       </c>
@@ -3273,7 +3279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>55</v>
       </c>
@@ -3296,7 +3302,7 @@
         <v>74438324012</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>56</v>
       </c>
@@ -3319,7 +3325,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>57</v>
       </c>
@@ -3342,7 +3348,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>58</v>
       </c>
@@ -3365,7 +3371,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>59</v>
       </c>
@@ -3388,7 +3394,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>60</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>61</v>
       </c>
@@ -3434,7 +3440,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>62</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>63</v>
       </c>
@@ -3480,7 +3486,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>64</v>
       </c>
@@ -3503,7 +3509,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>65</v>
       </c>
@@ -3526,7 +3532,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>66</v>
       </c>
@@ -3549,7 +3555,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>67</v>
       </c>
@@ -3572,7 +3578,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>68</v>
       </c>
@@ -3595,7 +3601,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>69</v>
       </c>
@@ -3618,7 +3624,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>70</v>
       </c>
@@ -3641,7 +3647,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>71</v>
       </c>
@@ -3664,7 +3670,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>72</v>
       </c>
@@ -3687,7 +3693,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>73</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>74</v>
       </c>
@@ -3733,7 +3739,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>75</v>
       </c>
@@ -3756,7 +3762,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>76</v>
       </c>
@@ -3779,7 +3785,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>77</v>
       </c>
@@ -3802,7 +3808,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>78</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>79</v>
       </c>
@@ -3848,7 +3854,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>80</v>
       </c>
@@ -3871,7 +3877,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>81</v>
       </c>
@@ -3894,7 +3900,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>82</v>
       </c>
@@ -3917,7 +3923,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>83</v>
       </c>
@@ -3940,7 +3946,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>84</v>
       </c>
@@ -3963,7 +3969,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>85</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>86</v>
       </c>
@@ -4009,7 +4015,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>87</v>
       </c>
@@ -4032,7 +4038,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>88</v>
       </c>
@@ -4055,7 +4061,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>89</v>
       </c>
@@ -4081,7 +4087,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>90</v>
       </c>
@@ -4104,7 +4110,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>91</v>
       </c>
@@ -4130,7 +4136,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>92</v>
       </c>
@@ -4153,7 +4159,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>93</v>
       </c>
@@ -4176,7 +4182,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>94</v>
       </c>
@@ -4199,7 +4205,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>95</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>96</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>97</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>98</v>
       </c>
@@ -4291,7 +4297,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>99</v>
       </c>
@@ -4314,7 +4320,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>100</v>
       </c>
@@ -4337,7 +4343,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>101</v>
       </c>

</xml_diff>